<commit_message>
CRM table now xtable and LaTeX.
</commit_message>
<xml_diff>
--- a/chapters/ch09-Agriculture/datasets/Food CO2.xlsx
+++ b/chapters/ch09-Agriculture/datasets/Food CO2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MCBook2021/chapters/ch09-Agriculture/datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48F586D-6F80-374D-8F3B-2A87FF4D1BD9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF51D07D-A627-F84C-BCA0-3981D63C17D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18720" yWindow="1160" windowWidth="27640" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18720" yWindow="1160" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data to plot" sheetId="2" r:id="rId1"/>
@@ -979,7 +979,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5878718-E362-0A40-85C8-E5A727E4EF17}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
@@ -1144,8 +1144,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>